<commit_message>
se edita archivo ejemplo
</commit_message>
<xml_diff>
--- a/ejemplos_clase/Test_Case_Ejempl_clase.xlsx
+++ b/ejemplos_clase/Test_Case_Ejempl_clase.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ttt</t>
   </si>
 </sst>
 </file>
@@ -190,18 +193,18 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="17.29"/>
   </cols>
@@ -293,7 +296,9 @@
       <c r="A8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>

</xml_diff>